<commit_message>
ajustements propagation d'incertitude à 150 N
</commit_message>
<xml_diff>
--- a/bin/Propagation_Erreurs.xlsx
+++ b/bin/Propagation_Erreurs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\picco\Desktop\POLYMTL - H2024\MEC8211\Projet Final\MEC8211ProjetFinal\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DD5B4B-D5F5-460E-8461-49A4BF1714D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B3CF19-61B7-496A-908B-6DFFFEA86A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CDE8206E-530D-4A97-96C2-0FF94BFE57EF}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{CDE8206E-530D-4A97-96C2-0FF94BFE57EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Propagation" sheetId="1" r:id="rId1"/>
@@ -7834,7 +7834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE228C3A-9E70-450D-A6BE-44C05C078166}">
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -11027,8 +11027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C1EA4D-B64D-465D-B394-8102E75D07B9}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11069,7 +11069,9 @@
       <c r="I2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="35"/>
+      <c r="J2" s="35">
+        <v>17.86</v>
+      </c>
       <c r="M2" t="s">
         <v>16</v>
       </c>
@@ -11078,7 +11080,7 @@
       </c>
       <c r="P2" s="37">
         <f>J6-J11</f>
-        <v>-3.2576155865158674</v>
+        <v>-2.2376155865158678</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -11096,7 +11098,7 @@
       </c>
       <c r="P3" s="37">
         <f>J6+J11</f>
-        <v>3.2576155865158674</v>
+        <v>4.2776155865158669</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -11108,7 +11110,9 @@
       <c r="I4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="35"/>
+      <c r="J4" s="35">
+        <v>18.88</v>
+      </c>
       <c r="P4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -11132,7 +11136,7 @@
       </c>
       <c r="J6" s="35">
         <f>J4-J2</f>
-        <v>0</v>
+        <v>1.0199999999999996</v>
       </c>
       <c r="P6" s="4"/>
     </row>

</xml_diff>